<commit_message>
use different DB connections for the timed services
</commit_message>
<xml_diff>
--- a/Useful/VariableConverted.xlsx
+++ b/Useful/VariableConverted.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owenholloway/Code/C#/NemTracker/Useful/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62395263-8813-F345-AF76-DEB96976AAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8C0E8-D465-2740-A00F-5230594556AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41220" yWindow="4320" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{DA1AE469-F5E3-5145-9063-675D6E6FF3EB}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{DA1AE469-F5E3-5145-9063-675D6E6FF3EB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Working" sheetId="1" r:id="rId1"/>
+    <sheet name="CSV Consume" sheetId="2" r:id="rId2"/>
     <sheet name="TO SQL" sheetId="3" r:id="rId3"/>
+    <sheet name="dto -&gt; obj" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1011,48 +1012,12 @@
     <t>excess_generation</t>
   </si>
   <si>
-    <t>raise_6_sec_rrp</t>
-  </si>
-  <si>
-    <t>raise_6_sec_rop</t>
-  </si>
-  <si>
-    <t>raise_60_sec_rrp</t>
-  </si>
-  <si>
-    <t>raise_60_sec_rop</t>
-  </si>
-  <si>
-    <t>raise_5_min_rrp</t>
-  </si>
-  <si>
-    <t>raise_5_min_rop</t>
-  </si>
-  <si>
     <t>raise_reg_rrp</t>
   </si>
   <si>
     <t>raise_reg_rop</t>
   </si>
   <si>
-    <t>lower_6_sec_rrp</t>
-  </si>
-  <si>
-    <t>lower_6_sec_rop</t>
-  </si>
-  <si>
-    <t>lower_60_sec_rrp</t>
-  </si>
-  <si>
-    <t>lower_60_sec_rop</t>
-  </si>
-  <si>
-    <t>lower_5_min_rrp</t>
-  </si>
-  <si>
-    <t>lower_5_min_rop</t>
-  </si>
-  <si>
     <t>lower_reg_rrp</t>
   </si>
   <si>
@@ -1074,96 +1039,6 @@
     <t>dispatchable_load</t>
   </si>
   <si>
-    <t>lower_5_min_dispatch</t>
-  </si>
-  <si>
-    <t>lower_5_min_import</t>
-  </si>
-  <si>
-    <t>lower_5_min_local_dispatch</t>
-  </si>
-  <si>
-    <t>lower_5_min_local_req</t>
-  </si>
-  <si>
-    <t>lower_5_min_req</t>
-  </si>
-  <si>
-    <t>lower_60_sec_dispatch</t>
-  </si>
-  <si>
-    <t>lower_60_sec_import</t>
-  </si>
-  <si>
-    <t>lower_60_sec_local_dispatch</t>
-  </si>
-  <si>
-    <t>lower_60_sec_local_req</t>
-  </si>
-  <si>
-    <t>lower_60_sec_req</t>
-  </si>
-  <si>
-    <t>lower_6_sec_dispatch</t>
-  </si>
-  <si>
-    <t>lower_6_sec_import</t>
-  </si>
-  <si>
-    <t>lower_6_sec_local_dispatch</t>
-  </si>
-  <si>
-    <t>lower_6_sec_local_req</t>
-  </si>
-  <si>
-    <t>lower_6_sec_req</t>
-  </si>
-  <si>
-    <t>raise_5_min_dispatch</t>
-  </si>
-  <si>
-    <t>raise_5_min_import</t>
-  </si>
-  <si>
-    <t>raise_5_min_local_dispatch</t>
-  </si>
-  <si>
-    <t>raise_5_min_local_req</t>
-  </si>
-  <si>
-    <t>raise_5_min_req</t>
-  </si>
-  <si>
-    <t>raise_60_sec_dispatch</t>
-  </si>
-  <si>
-    <t>raise_60_sec_import</t>
-  </si>
-  <si>
-    <t>raise_60_sec_local_dispatch</t>
-  </si>
-  <si>
-    <t>raise_60_sec_local_req</t>
-  </si>
-  <si>
-    <t>raise_60_sec_req</t>
-  </si>
-  <si>
-    <t>raise_6_sec_dispatch</t>
-  </si>
-  <si>
-    <t>raise_6_sec_import</t>
-  </si>
-  <si>
-    <t>raise_6_sec_local_dispatch</t>
-  </si>
-  <si>
-    <t>raise_6_sec_local_req</t>
-  </si>
-  <si>
-    <t>raise_6_sec_req</t>
-  </si>
-  <si>
     <t>aggregate_dispatch_error</t>
   </si>
   <si>
@@ -1203,54 +1078,18 @@
     <t>raise_reg_req</t>
   </si>
   <si>
-    <t>raise_5_min_local_violation</t>
-  </si>
-  <si>
     <t>raise_reg_local_violation</t>
   </si>
   <si>
-    <t>raise_60_sec_local_violation</t>
-  </si>
-  <si>
-    <t>raise_6_sec_local_violation</t>
-  </si>
-  <si>
-    <t>lower_5_min_local_violation</t>
-  </si>
-  <si>
     <t>lower_reg_local_violation</t>
   </si>
   <si>
-    <t>lower_60_sec_local_violation</t>
-  </si>
-  <si>
-    <t>lower_6_sec_local_violation</t>
-  </si>
-  <si>
-    <t>raise_5_min_violation</t>
-  </si>
-  <si>
     <t>raise_reg_violation</t>
   </si>
   <si>
-    <t>raise_60_sec_violation</t>
-  </si>
-  <si>
-    <t>raise_6_sec_violation</t>
-  </si>
-  <si>
-    <t>lower_5_min_violation</t>
-  </si>
-  <si>
     <t>lower_reg_violation</t>
   </si>
   <si>
-    <t>lower_60_sec_violation</t>
-  </si>
-  <si>
-    <t>lower_6_sec_violation</t>
-  </si>
-  <si>
     <t>last_changed</t>
   </si>
   <si>
@@ -1372,6 +1211,168 @@
   </si>
   <si>
     <t>net_interchange</t>
+  </si>
+  <si>
+    <t>raise6_sec_rrp</t>
+  </si>
+  <si>
+    <t>raise6_sec_rop</t>
+  </si>
+  <si>
+    <t>raise60_sec_rrp</t>
+  </si>
+  <si>
+    <t>raise60_sec_rop</t>
+  </si>
+  <si>
+    <t>raise5_min_rrp</t>
+  </si>
+  <si>
+    <t>raise5_min_rop</t>
+  </si>
+  <si>
+    <t>lower6_sec_rrp</t>
+  </si>
+  <si>
+    <t>lower6_sec_rop</t>
+  </si>
+  <si>
+    <t>lower60_sec_rrp</t>
+  </si>
+  <si>
+    <t>lower60_sec_rop</t>
+  </si>
+  <si>
+    <t>lower5_min_rrp</t>
+  </si>
+  <si>
+    <t>lower5_min_rop</t>
+  </si>
+  <si>
+    <t>lower5_min_dispatch</t>
+  </si>
+  <si>
+    <t>lower5_min_import</t>
+  </si>
+  <si>
+    <t>lower5_min_local_dispatch</t>
+  </si>
+  <si>
+    <t>lower5_min_local_req</t>
+  </si>
+  <si>
+    <t>lower5_min_req</t>
+  </si>
+  <si>
+    <t>lower60_sec_dispatch</t>
+  </si>
+  <si>
+    <t>lower60_sec_import</t>
+  </si>
+  <si>
+    <t>lower60_sec_local_dispatch</t>
+  </si>
+  <si>
+    <t>lower60_sec_local_req</t>
+  </si>
+  <si>
+    <t>lower60_sec_req</t>
+  </si>
+  <si>
+    <t>lower6_sec_dispatch</t>
+  </si>
+  <si>
+    <t>lower6_sec_import</t>
+  </si>
+  <si>
+    <t>lower6_sec_local_dispatch</t>
+  </si>
+  <si>
+    <t>lower6_sec_local_req</t>
+  </si>
+  <si>
+    <t>lower6_sec_req</t>
+  </si>
+  <si>
+    <t>raise5_min_dispatch</t>
+  </si>
+  <si>
+    <t>raise5_min_import</t>
+  </si>
+  <si>
+    <t>raise5_min_local_dispatch</t>
+  </si>
+  <si>
+    <t>raise5_min_local_req</t>
+  </si>
+  <si>
+    <t>raise5_min_req</t>
+  </si>
+  <si>
+    <t>raise60_sec_dispatch</t>
+  </si>
+  <si>
+    <t>raise60_sec_import</t>
+  </si>
+  <si>
+    <t>raise60_sec_local_dispatch</t>
+  </si>
+  <si>
+    <t>raise60_sec_local_req</t>
+  </si>
+  <si>
+    <t>raise60_sec_req</t>
+  </si>
+  <si>
+    <t>raise6_sec_dispatch</t>
+  </si>
+  <si>
+    <t>raise6_sec_import</t>
+  </si>
+  <si>
+    <t>raise6_sec_local_dispatch</t>
+  </si>
+  <si>
+    <t>raise6_sec_local_req</t>
+  </si>
+  <si>
+    <t>raise6_sec_req</t>
+  </si>
+  <si>
+    <t>raise5_min_local_violation</t>
+  </si>
+  <si>
+    <t>raise60_sec_local_violation</t>
+  </si>
+  <si>
+    <t>raise6_sec_local_violation</t>
+  </si>
+  <si>
+    <t>lower5_min_local_violation</t>
+  </si>
+  <si>
+    <t>lower60_sec_local_violation</t>
+  </si>
+  <si>
+    <t>lower6_sec_local_violation</t>
+  </si>
+  <si>
+    <t>raise5_min_violation</t>
+  </si>
+  <si>
+    <t>raise60_sec_violation</t>
+  </si>
+  <si>
+    <t>raise6_sec_violation</t>
+  </si>
+  <si>
+    <t>lower5_min_violation</t>
+  </si>
+  <si>
+    <t>lower60_sec_violation</t>
+  </si>
+  <si>
+    <t>lower6_sec_violation</t>
   </si>
 </sst>
 </file>
@@ -6395,7 +6396,7 @@
   <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J104"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6435,10 +6436,10 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" t="s">
-        <v>419</v>
+        <v>365</v>
       </c>
       <c r="T1" t="s">
-        <v>420</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -6473,10 +6474,10 @@
         <v>run_time date,</v>
       </c>
       <c r="S2" t="s">
-        <v>427</v>
+        <v>373</v>
       </c>
       <c r="T2" t="s">
-        <v>426</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -6511,10 +6512,10 @@
         <v>interval date,</v>
       </c>
       <c r="S3" t="s">
-        <v>429</v>
+        <v>375</v>
       </c>
       <c r="T3" t="s">
-        <v>428</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -6549,10 +6550,10 @@
         <v>region smallint,</v>
       </c>
       <c r="S4" t="s">
-        <v>431</v>
+        <v>377</v>
       </c>
       <c r="T4" t="s">
-        <v>430</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -6587,10 +6588,10 @@
         <v>rrp double precision,</v>
       </c>
       <c r="S5" t="s">
-        <v>423</v>
+        <v>369</v>
       </c>
       <c r="T5" t="s">
-        <v>432</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -6625,10 +6626,10 @@
         <v>rop double precision,</v>
       </c>
       <c r="S6" t="s">
-        <v>434</v>
+        <v>380</v>
       </c>
       <c r="T6" t="s">
-        <v>433</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -6663,10 +6664,10 @@
         <v>excess_generation double precision,</v>
       </c>
       <c r="S7" t="s">
-        <v>421</v>
+        <v>367</v>
       </c>
       <c r="T7" t="s">
-        <v>425</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -6690,7 +6691,7 @@
         <v>Raise6SecRrp</v>
       </c>
       <c r="G8" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -6698,13 +6699,13 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_rrp double precision,</v>
+        <v>raise6_sec_rrp double precision,</v>
       </c>
       <c r="S8" t="s">
-        <v>436</v>
+        <v>382</v>
       </c>
       <c r="T8" t="s">
-        <v>435</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -6728,7 +6729,7 @@
         <v>Raise6SecRop</v>
       </c>
       <c r="G9" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -6736,13 +6737,13 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_rop double precision,</v>
+        <v>raise6_sec_rop double precision,</v>
       </c>
       <c r="S9" t="s">
-        <v>438</v>
+        <v>384</v>
       </c>
       <c r="T9" t="s">
-        <v>437</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -6766,7 +6767,7 @@
         <v>Raise60SecRrp</v>
       </c>
       <c r="G10" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -6774,13 +6775,13 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_rrp double precision,</v>
+        <v>raise60_sec_rrp double precision,</v>
       </c>
       <c r="S10" t="s">
-        <v>422</v>
+        <v>368</v>
       </c>
       <c r="T10" t="s">
-        <v>424</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -6804,7 +6805,7 @@
         <v>Raise60SecRop</v>
       </c>
       <c r="G11" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -6812,13 +6813,13 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_rop double precision,</v>
+        <v>raise60_sec_rop double precision,</v>
       </c>
       <c r="S11" t="s">
-        <v>427</v>
+        <v>373</v>
       </c>
       <c r="T11" t="s">
-        <v>439</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -6842,7 +6843,7 @@
         <v>Raise5MinRrp</v>
       </c>
       <c r="G12" t="s">
-        <v>328</v>
+        <v>395</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -6850,13 +6851,13 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_rrp double precision,</v>
+        <v>raise5_min_rrp double precision,</v>
       </c>
       <c r="S12" t="s">
-        <v>440</v>
+        <v>386</v>
       </c>
       <c r="T12" t="s">
-        <v>428</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -6880,7 +6881,7 @@
         <v>Raise5MinRop</v>
       </c>
       <c r="G13" t="s">
-        <v>329</v>
+        <v>396</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -6888,7 +6889,7 @@
       </c>
       <c r="J13" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_rop double precision,</v>
+        <v>raise5_min_rop double precision,</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -6912,7 +6913,7 @@
         <v>RaiseRegRrp</v>
       </c>
       <c r="G14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -6944,7 +6945,7 @@
         <v>RaiseRegRop</v>
       </c>
       <c r="G15" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -6976,7 +6977,7 @@
         <v>Lower6SecRrp</v>
       </c>
       <c r="G16" t="s">
-        <v>332</v>
+        <v>397</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -6984,7 +6985,7 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_rrp double precision,</v>
+        <v>lower6_sec_rrp double precision,</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -7008,7 +7009,7 @@
         <v>Lower6SecRop</v>
       </c>
       <c r="G17" t="s">
-        <v>333</v>
+        <v>398</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -7016,7 +7017,7 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_rop double precision,</v>
+        <v>lower6_sec_rop double precision,</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -7040,7 +7041,7 @@
         <v>Lower60SecRrp</v>
       </c>
       <c r="G18" t="s">
-        <v>334</v>
+        <v>399</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -7048,7 +7049,7 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_rrp double precision,</v>
+        <v>lower60_sec_rrp double precision,</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -7072,7 +7073,7 @@
         <v>Lower60SecRop</v>
       </c>
       <c r="G19" t="s">
-        <v>335</v>
+        <v>400</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -7080,7 +7081,7 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_rop double precision,</v>
+        <v>lower60_sec_rop double precision,</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -7104,7 +7105,7 @@
         <v>Lower5MinRrp</v>
       </c>
       <c r="G20" t="s">
-        <v>336</v>
+        <v>401</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -7112,7 +7113,7 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_rrp double precision,</v>
+        <v>lower5_min_rrp double precision,</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -7136,7 +7137,7 @@
         <v>Lower5MinRop</v>
       </c>
       <c r="G21" t="s">
-        <v>337</v>
+        <v>402</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -7144,7 +7145,7 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_rop double precision,</v>
+        <v>lower5_min_rop double precision,</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -7168,7 +7169,7 @@
         <v>LowerRegRrp</v>
       </c>
       <c r="G22" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -7200,7 +7201,7 @@
         <v>LowerRegRop</v>
       </c>
       <c r="G23" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -7213,7 +7214,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>387</v>
       </c>
       <c r="B24">
         <f t="shared" si="1"/>
@@ -7232,7 +7233,7 @@
         <v>TotalDemand</v>
       </c>
       <c r="G24" t="s">
-        <v>443</v>
+        <v>389</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -7264,7 +7265,7 @@
         <v>AvailableGeneration</v>
       </c>
       <c r="G25" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -7296,7 +7297,7 @@
         <v>AvailableLoad</v>
       </c>
       <c r="G26" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -7328,7 +7329,7 @@
         <v>DemandForecast</v>
       </c>
       <c r="G27" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -7360,7 +7361,7 @@
         <v>DispatchableGeneration</v>
       </c>
       <c r="G28" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -7392,7 +7393,7 @@
         <v>DispatchableLoad</v>
       </c>
       <c r="G29" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -7405,7 +7406,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>442</v>
+        <v>388</v>
       </c>
       <c r="B30">
         <f t="shared" si="1"/>
@@ -7424,7 +7425,7 @@
         <v>NetInterchange</v>
       </c>
       <c r="G30" t="s">
-        <v>444</v>
+        <v>390</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -7456,7 +7457,7 @@
         <v>Lower5MinDispatch</v>
       </c>
       <c r="G31" t="s">
-        <v>345</v>
+        <v>403</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -7464,7 +7465,7 @@
       </c>
       <c r="J31" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_dispatch double precision,</v>
+        <v>lower5_min_dispatch double precision,</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -7488,7 +7489,7 @@
         <v>Lower5MinImport</v>
       </c>
       <c r="G32" t="s">
-        <v>346</v>
+        <v>404</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -7496,7 +7497,7 @@
       </c>
       <c r="J32" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_import double precision,</v>
+        <v>lower5_min_import double precision,</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -7520,7 +7521,7 @@
         <v>Lower5MinLocalDispatch</v>
       </c>
       <c r="G33" t="s">
-        <v>347</v>
+        <v>405</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -7528,7 +7529,7 @@
       </c>
       <c r="J33" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_local_dispatch double precision,</v>
+        <v>lower5_min_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -7552,7 +7553,7 @@
         <v>Lower5MinLocalReq</v>
       </c>
       <c r="G34" t="s">
-        <v>348</v>
+        <v>406</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -7560,7 +7561,7 @@
       </c>
       <c r="J34" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_local_req double precision,</v>
+        <v>lower5_min_local_req double precision,</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -7584,7 +7585,7 @@
         <v>Lower5MinReq</v>
       </c>
       <c r="G35" t="s">
-        <v>349</v>
+        <v>407</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -7592,7 +7593,7 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="5"/>
-        <v>lower_5_min_req double precision,</v>
+        <v>lower5_min_req double precision,</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -7616,7 +7617,7 @@
         <v>Lower60SecDispatch</v>
       </c>
       <c r="G36" t="s">
-        <v>350</v>
+        <v>408</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -7624,7 +7625,7 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_dispatch double precision,</v>
+        <v>lower60_sec_dispatch double precision,</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -7648,7 +7649,7 @@
         <v>Lower60SecImport</v>
       </c>
       <c r="G37" t="s">
-        <v>351</v>
+        <v>409</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -7656,7 +7657,7 @@
       </c>
       <c r="J37" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_import double precision,</v>
+        <v>lower60_sec_import double precision,</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -7680,7 +7681,7 @@
         <v>Lower60SecLocalDispatch</v>
       </c>
       <c r="G38" t="s">
-        <v>352</v>
+        <v>410</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -7688,7 +7689,7 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_local_dispatch double precision,</v>
+        <v>lower60_sec_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -7712,7 +7713,7 @@
         <v>Lower60SecLocalReq</v>
       </c>
       <c r="G39" t="s">
-        <v>353</v>
+        <v>411</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -7720,7 +7721,7 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_local_req double precision,</v>
+        <v>lower60_sec_local_req double precision,</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -7744,7 +7745,7 @@
         <v>Lower60SecReq</v>
       </c>
       <c r="G40" t="s">
-        <v>354</v>
+        <v>412</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -7752,7 +7753,7 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="5"/>
-        <v>lower_60_sec_req double precision,</v>
+        <v>lower60_sec_req double precision,</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -7776,7 +7777,7 @@
         <v>Lower6SecDispatch</v>
       </c>
       <c r="G41" t="s">
-        <v>355</v>
+        <v>413</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -7784,7 +7785,7 @@
       </c>
       <c r="J41" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_dispatch double precision,</v>
+        <v>lower6_sec_dispatch double precision,</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -7808,7 +7809,7 @@
         <v>Lower6SecImport</v>
       </c>
       <c r="G42" t="s">
-        <v>356</v>
+        <v>414</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -7816,7 +7817,7 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_import double precision,</v>
+        <v>lower6_sec_import double precision,</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -7840,7 +7841,7 @@
         <v>Lower6SecLocalDispatch</v>
       </c>
       <c r="G43" t="s">
-        <v>357</v>
+        <v>415</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -7848,7 +7849,7 @@
       </c>
       <c r="J43" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_local_dispatch double precision,</v>
+        <v>lower6_sec_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -7872,7 +7873,7 @@
         <v>Lower6SecLocalReq</v>
       </c>
       <c r="G44" t="s">
-        <v>358</v>
+        <v>416</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -7880,7 +7881,7 @@
       </c>
       <c r="J44" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_local_req double precision,</v>
+        <v>lower6_sec_local_req double precision,</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -7904,7 +7905,7 @@
         <v>Lower6SecReq</v>
       </c>
       <c r="G45" t="s">
-        <v>359</v>
+        <v>417</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -7912,7 +7913,7 @@
       </c>
       <c r="J45" t="str">
         <f t="shared" si="5"/>
-        <v>lower_6_sec_req double precision,</v>
+        <v>lower6_sec_req double precision,</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -7936,7 +7937,7 @@
         <v>Raise5MinDispatch</v>
       </c>
       <c r="G46" t="s">
-        <v>360</v>
+        <v>418</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -7944,7 +7945,7 @@
       </c>
       <c r="J46" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_dispatch double precision,</v>
+        <v>raise5_min_dispatch double precision,</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -7968,7 +7969,7 @@
         <v>Raise5MinImport</v>
       </c>
       <c r="G47" t="s">
-        <v>361</v>
+        <v>419</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -7976,7 +7977,7 @@
       </c>
       <c r="J47" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_import double precision,</v>
+        <v>raise5_min_import double precision,</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -8000,7 +8001,7 @@
         <v>Raise5MinLocalDispatch</v>
       </c>
       <c r="G48" t="s">
-        <v>362</v>
+        <v>420</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -8008,7 +8009,7 @@
       </c>
       <c r="J48" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_local_dispatch double precision,</v>
+        <v>raise5_min_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -8032,7 +8033,7 @@
         <v>Raise5MinLocalReq</v>
       </c>
       <c r="G49" t="s">
-        <v>363</v>
+        <v>421</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -8040,7 +8041,7 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_local_req double precision,</v>
+        <v>raise5_min_local_req double precision,</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -8064,7 +8065,7 @@
         <v>Raise5MinReq</v>
       </c>
       <c r="G50" t="s">
-        <v>364</v>
+        <v>422</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -8072,7 +8073,7 @@
       </c>
       <c r="J50" t="str">
         <f t="shared" si="5"/>
-        <v>raise_5_min_req double precision,</v>
+        <v>raise5_min_req double precision,</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -8096,7 +8097,7 @@
         <v>Raise60SecDispatch</v>
       </c>
       <c r="G51" t="s">
-        <v>365</v>
+        <v>423</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -8104,7 +8105,7 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_dispatch double precision,</v>
+        <v>raise60_sec_dispatch double precision,</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -8128,7 +8129,7 @@
         <v>Raise60SecImport</v>
       </c>
       <c r="G52" t="s">
-        <v>366</v>
+        <v>424</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -8136,7 +8137,7 @@
       </c>
       <c r="J52" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_import double precision,</v>
+        <v>raise60_sec_import double precision,</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -8160,7 +8161,7 @@
         <v>Raise60SecLocalDispatch</v>
       </c>
       <c r="G53" t="s">
-        <v>367</v>
+        <v>425</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -8168,7 +8169,7 @@
       </c>
       <c r="J53" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_local_dispatch double precision,</v>
+        <v>raise60_sec_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -8192,7 +8193,7 @@
         <v>Raise60SecLocalReq</v>
       </c>
       <c r="G54" t="s">
-        <v>368</v>
+        <v>426</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -8200,7 +8201,7 @@
       </c>
       <c r="J54" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_local_req double precision,</v>
+        <v>raise60_sec_local_req double precision,</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -8224,7 +8225,7 @@
         <v>Raise60SecReq</v>
       </c>
       <c r="G55" t="s">
-        <v>369</v>
+        <v>427</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -8232,7 +8233,7 @@
       </c>
       <c r="J55" t="str">
         <f t="shared" si="5"/>
-        <v>raise_60_sec_req double precision,</v>
+        <v>raise60_sec_req double precision,</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -8256,7 +8257,7 @@
         <v>Raise6SecDispatch</v>
       </c>
       <c r="G56" t="s">
-        <v>370</v>
+        <v>428</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -8264,7 +8265,7 @@
       </c>
       <c r="J56" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_dispatch double precision,</v>
+        <v>raise6_sec_dispatch double precision,</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -8288,7 +8289,7 @@
         <v>Raise6SecImport</v>
       </c>
       <c r="G57" t="s">
-        <v>371</v>
+        <v>429</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -8296,7 +8297,7 @@
       </c>
       <c r="J57" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_import double precision,</v>
+        <v>raise6_sec_import double precision,</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -8320,7 +8321,7 @@
         <v>Raise6SecLocalDispatch</v>
       </c>
       <c r="G58" t="s">
-        <v>372</v>
+        <v>430</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -8328,7 +8329,7 @@
       </c>
       <c r="J58" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_local_dispatch double precision,</v>
+        <v>raise6_sec_local_dispatch double precision,</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -8352,7 +8353,7 @@
         <v>Raise6SecLocalReq</v>
       </c>
       <c r="G59" t="s">
-        <v>373</v>
+        <v>431</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -8360,7 +8361,7 @@
       </c>
       <c r="J59" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_local_req double precision,</v>
+        <v>raise6_sec_local_req double precision,</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -8384,7 +8385,7 @@
         <v>Raise6SecReq</v>
       </c>
       <c r="G60" t="s">
-        <v>374</v>
+        <v>432</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -8392,7 +8393,7 @@
       </c>
       <c r="J60" t="str">
         <f t="shared" si="5"/>
-        <v>raise_6_sec_req double precision,</v>
+        <v>raise6_sec_req double precision,</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -8416,7 +8417,7 @@
         <v>AggregateDispatchError</v>
       </c>
       <c r="G61" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -8448,7 +8449,7 @@
         <v>InitialSupply</v>
       </c>
       <c r="G62" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -8480,7 +8481,7 @@
         <v>ClearedSupply</v>
       </c>
       <c r="G63" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -8512,7 +8513,7 @@
         <v>LowerRegImport</v>
       </c>
       <c r="G64" t="s">
-        <v>378</v>
+        <v>336</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -8544,7 +8545,7 @@
         <v>LowerRegDispatch</v>
       </c>
       <c r="G65" t="s">
-        <v>379</v>
+        <v>337</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -8576,7 +8577,7 @@
         <v>LowerRegLocalDispatch</v>
       </c>
       <c r="G66" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" ref="H66:H104" si="6">VLOOKUP(D66,$S$2:$T$20,2,FALSE)</f>
@@ -8608,7 +8609,7 @@
         <v>LowerRegLocalReq</v>
       </c>
       <c r="G67" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" si="6"/>
@@ -8640,7 +8641,7 @@
         <v>LowerRegReq</v>
       </c>
       <c r="G68" t="s">
-        <v>382</v>
+        <v>340</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="6"/>
@@ -8672,7 +8673,7 @@
         <v>RaiseRegImport</v>
       </c>
       <c r="G69" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="6"/>
@@ -8704,7 +8705,7 @@
         <v>RaiseRegDispatch</v>
       </c>
       <c r="G70" t="s">
-        <v>384</v>
+        <v>342</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="6"/>
@@ -8736,7 +8737,7 @@
         <v>RaiseRegLocalDispatch</v>
       </c>
       <c r="G71" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="6"/>
@@ -8768,7 +8769,7 @@
         <v>RaiseRegLocalReq</v>
       </c>
       <c r="G72" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="6"/>
@@ -8800,7 +8801,7 @@
         <v>RaiseRegReq</v>
       </c>
       <c r="G73" t="s">
-        <v>387</v>
+        <v>345</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="6"/>
@@ -8832,7 +8833,7 @@
         <v>Raise5MinLocalViolation</v>
       </c>
       <c r="G74" t="s">
-        <v>388</v>
+        <v>433</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="6"/>
@@ -8840,7 +8841,7 @@
       </c>
       <c r="J74" t="str">
         <f t="shared" si="11"/>
-        <v>raise_5_min_local_violation double precision,</v>
+        <v>raise5_min_local_violation double precision,</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -8864,7 +8865,7 @@
         <v>RaiseRegLocalViolation</v>
       </c>
       <c r="G75" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="6"/>
@@ -8896,7 +8897,7 @@
         <v>Raise60SecLocalViolation</v>
       </c>
       <c r="G76" t="s">
-        <v>390</v>
+        <v>434</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="6"/>
@@ -8904,7 +8905,7 @@
       </c>
       <c r="J76" t="str">
         <f t="shared" si="11"/>
-        <v>raise_60_sec_local_violation double precision,</v>
+        <v>raise60_sec_local_violation double precision,</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -8928,7 +8929,7 @@
         <v>Raise6SecLocalViolation</v>
       </c>
       <c r="G77" t="s">
-        <v>391</v>
+        <v>435</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="6"/>
@@ -8936,7 +8937,7 @@
       </c>
       <c r="J77" t="str">
         <f t="shared" si="11"/>
-        <v>raise_6_sec_local_violation double precision,</v>
+        <v>raise6_sec_local_violation double precision,</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -8960,7 +8961,7 @@
         <v>Lower5MinLocalViolation</v>
       </c>
       <c r="G78" t="s">
-        <v>392</v>
+        <v>436</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="6"/>
@@ -8968,7 +8969,7 @@
       </c>
       <c r="J78" t="str">
         <f t="shared" si="11"/>
-        <v>lower_5_min_local_violation double precision,</v>
+        <v>lower5_min_local_violation double precision,</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -8992,7 +8993,7 @@
         <v>LowerRegLocalViolation</v>
       </c>
       <c r="G79" t="s">
-        <v>393</v>
+        <v>347</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="6"/>
@@ -9024,7 +9025,7 @@
         <v>Lower60SecLocalViolation</v>
       </c>
       <c r="G80" t="s">
-        <v>394</v>
+        <v>437</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="6"/>
@@ -9032,7 +9033,7 @@
       </c>
       <c r="J80" t="str">
         <f t="shared" si="11"/>
-        <v>lower_60_sec_local_violation double precision,</v>
+        <v>lower60_sec_local_violation double precision,</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -9056,7 +9057,7 @@
         <v>Lower6SecLocalViolation</v>
       </c>
       <c r="G81" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="6"/>
@@ -9064,7 +9065,7 @@
       </c>
       <c r="J81" t="str">
         <f t="shared" si="11"/>
-        <v>lower_6_sec_local_violation double precision,</v>
+        <v>lower6_sec_local_violation double precision,</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -9088,7 +9089,7 @@
         <v>Raise5MinViolation</v>
       </c>
       <c r="G82" t="s">
-        <v>396</v>
+        <v>439</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="6"/>
@@ -9096,7 +9097,7 @@
       </c>
       <c r="J82" t="str">
         <f t="shared" si="11"/>
-        <v>raise_5_min_violation double precision,</v>
+        <v>raise5_min_violation double precision,</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -9120,7 +9121,7 @@
         <v>RaiseRegViolation</v>
       </c>
       <c r="G83" t="s">
-        <v>397</v>
+        <v>348</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="6"/>
@@ -9152,7 +9153,7 @@
         <v>Raise60SecViolation</v>
       </c>
       <c r="G84" t="s">
-        <v>398</v>
+        <v>440</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="6"/>
@@ -9160,7 +9161,7 @@
       </c>
       <c r="J84" t="str">
         <f t="shared" si="11"/>
-        <v>raise_60_sec_violation double precision,</v>
+        <v>raise60_sec_violation double precision,</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
@@ -9184,7 +9185,7 @@
         <v>Raise6SecViolation</v>
       </c>
       <c r="G85" t="s">
-        <v>399</v>
+        <v>441</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="6"/>
@@ -9192,7 +9193,7 @@
       </c>
       <c r="J85" t="str">
         <f t="shared" si="11"/>
-        <v>raise_6_sec_violation double precision,</v>
+        <v>raise6_sec_violation double precision,</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -9216,7 +9217,7 @@
         <v>Lower5MinViolation</v>
       </c>
       <c r="G86" t="s">
-        <v>400</v>
+        <v>442</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="6"/>
@@ -9224,7 +9225,7 @@
       </c>
       <c r="J86" t="str">
         <f t="shared" si="11"/>
-        <v>lower_5_min_violation double precision,</v>
+        <v>lower5_min_violation double precision,</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
@@ -9248,7 +9249,7 @@
         <v>LowerRegViolation</v>
       </c>
       <c r="G87" t="s">
-        <v>401</v>
+        <v>349</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="6"/>
@@ -9280,7 +9281,7 @@
         <v>Lower60SecViolation</v>
       </c>
       <c r="G88" t="s">
-        <v>402</v>
+        <v>443</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="6"/>
@@ -9288,7 +9289,7 @@
       </c>
       <c r="J88" t="str">
         <f t="shared" si="11"/>
-        <v>lower_60_sec_violation double precision,</v>
+        <v>lower60_sec_violation double precision,</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -9312,7 +9313,7 @@
         <v>Lower6SecViolation</v>
       </c>
       <c r="G89" t="s">
-        <v>403</v>
+        <v>444</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="6"/>
@@ -9320,7 +9321,7 @@
       </c>
       <c r="J89" t="str">
         <f t="shared" si="11"/>
-        <v>lower_6_sec_violation double precision,</v>
+        <v>lower6_sec_violation double precision,</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
@@ -9344,7 +9345,7 @@
         <v>LastChanged</v>
       </c>
       <c r="G90" t="s">
-        <v>404</v>
+        <v>350</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="6"/>
@@ -9376,7 +9377,7 @@
         <v>TotalIntermittentGeneration</v>
       </c>
       <c r="G91" t="s">
-        <v>405</v>
+        <v>351</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="6"/>
@@ -9408,7 +9409,7 @@
         <v>DemandAndNonSchedgen</v>
       </c>
       <c r="G92" t="s">
-        <v>406</v>
+        <v>352</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="6"/>
@@ -9440,7 +9441,7 @@
         <v>Uigf</v>
       </c>
       <c r="G93" t="s">
-        <v>407</v>
+        <v>353</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="6"/>
@@ -9472,7 +9473,7 @@
         <v>SemiScheduleClearedMw</v>
       </c>
       <c r="G94" t="s">
-        <v>408</v>
+        <v>354</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="6"/>
@@ -9504,7 +9505,7 @@
         <v>SemiScheduleComplianceMw</v>
       </c>
       <c r="G95" t="s">
-        <v>409</v>
+        <v>355</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="6"/>
@@ -9536,7 +9537,7 @@
         <v>SsSolarUigf</v>
       </c>
       <c r="G96" t="s">
-        <v>410</v>
+        <v>356</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="6"/>
@@ -9568,7 +9569,7 @@
         <v>SsWindUigf</v>
       </c>
       <c r="G97" t="s">
-        <v>411</v>
+        <v>357</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="6"/>
@@ -9600,7 +9601,7 @@
         <v>SsSolarClearedMw</v>
       </c>
       <c r="G98" t="s">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="6"/>
@@ -9632,7 +9633,7 @@
         <v>SsWindClearedMw</v>
       </c>
       <c r="G99" t="s">
-        <v>413</v>
+        <v>359</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="6"/>
@@ -9664,7 +9665,7 @@
         <v>SsSolarComplianceMw</v>
       </c>
       <c r="G100" t="s">
-        <v>414</v>
+        <v>360</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="6"/>
@@ -9696,7 +9697,7 @@
         <v>SsWindComplianceMw</v>
       </c>
       <c r="G101" t="s">
-        <v>415</v>
+        <v>361</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="6"/>
@@ -9728,7 +9729,7 @@
         <v>WdrInitialMw</v>
       </c>
       <c r="G102" t="s">
-        <v>416</v>
+        <v>362</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="6"/>
@@ -9760,7 +9761,7 @@
         <v>WdrAvailable</v>
       </c>
       <c r="G103" t="s">
-        <v>417</v>
+        <v>363</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="6"/>
@@ -9792,7 +9793,7 @@
         <v>WdrDispatched</v>
       </c>
       <c r="G104" t="s">
-        <v>418</v>
+        <v>364</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="6"/>
@@ -9801,6 +9802,1056 @@
       <c r="J104" t="str">
         <f t="shared" si="11"/>
         <v>wdr_dispatched double precision,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C23C844-F8C1-7647-9D7E-CC7573F8BDAE}">
+  <dimension ref="A2:B104"/>
+  <sheetViews>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>'TO SQL'!E2</f>
+        <v>RunTime</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT(A2," = ","dto.",A2,";")</f>
+        <v>RunTime = dto.RunTime;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>'TO SQL'!E3</f>
+        <v>Interval</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">_xlfn.CONCAT(A3," = ","dto.",A3,";")</f>
+        <v>Interval = dto.Interval;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>'TO SQL'!E4</f>
+        <v>Region</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Region = dto.Region;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>'TO SQL'!E5</f>
+        <v>Rrp</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Rrp = dto.Rrp;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>'TO SQL'!E6</f>
+        <v>Rop</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Rop = dto.Rop;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>'TO SQL'!E7</f>
+        <v>ExcessGeneration</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>ExcessGeneration = dto.ExcessGeneration;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>'TO SQL'!E8</f>
+        <v>Raise6SecRrp</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecRrp = dto.Raise6SecRrp;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>'TO SQL'!E9</f>
+        <v>Raise6SecRop</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecRop = dto.Raise6SecRop;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>'TO SQL'!E10</f>
+        <v>Raise60SecRrp</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecRrp = dto.Raise60SecRrp;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>'TO SQL'!E11</f>
+        <v>Raise60SecRop</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecRop = dto.Raise60SecRop;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>'TO SQL'!E12</f>
+        <v>Raise5MinRrp</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinRrp = dto.Raise5MinRrp;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>'TO SQL'!E13</f>
+        <v>Raise5MinRop</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinRop = dto.Raise5MinRop;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>'TO SQL'!E14</f>
+        <v>RaiseRegRrp</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>RaiseRegRrp = dto.RaiseRegRrp;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>'TO SQL'!E15</f>
+        <v>RaiseRegRop</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>RaiseRegRop = dto.RaiseRegRop;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>'TO SQL'!E16</f>
+        <v>Lower6SecRrp</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecRrp = dto.Lower6SecRrp;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>'TO SQL'!E17</f>
+        <v>Lower6SecRop</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecRop = dto.Lower6SecRop;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f>'TO SQL'!E18</f>
+        <v>Lower60SecRrp</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecRrp = dto.Lower60SecRrp;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f>'TO SQL'!E19</f>
+        <v>Lower60SecRop</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecRop = dto.Lower60SecRop;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f>'TO SQL'!E20</f>
+        <v>Lower5MinRrp</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinRrp = dto.Lower5MinRrp;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f>'TO SQL'!E21</f>
+        <v>Lower5MinRop</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinRop = dto.Lower5MinRop;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f>'TO SQL'!E22</f>
+        <v>LowerRegRrp</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>LowerRegRrp = dto.LowerRegRrp;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f>'TO SQL'!E23</f>
+        <v>LowerRegRop</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>LowerRegRop = dto.LowerRegRop;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>'TO SQL'!E24</f>
+        <v>TotalDemand</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>TotalDemand = dto.TotalDemand;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>'TO SQL'!E25</f>
+        <v>AvailableGeneration</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>AvailableGeneration = dto.AvailableGeneration;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>'TO SQL'!E26</f>
+        <v>AvailableLoad</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>AvailableLoad = dto.AvailableLoad;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>'TO SQL'!E27</f>
+        <v>DemandForecast</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>DemandForecast = dto.DemandForecast;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f>'TO SQL'!E28</f>
+        <v>DispatchableGeneration</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>DispatchableGeneration = dto.DispatchableGeneration;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f>'TO SQL'!E29</f>
+        <v>DispatchableLoad</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>DispatchableLoad = dto.DispatchableLoad;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f>'TO SQL'!E30</f>
+        <v>NetInterchange</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>NetInterchange = dto.NetInterchange;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>'TO SQL'!E31</f>
+        <v>Lower5MinDispatch</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinDispatch = dto.Lower5MinDispatch;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>'TO SQL'!E32</f>
+        <v>Lower5MinImport</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinImport = dto.Lower5MinImport;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>'TO SQL'!E33</f>
+        <v>Lower5MinLocalDispatch</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinLocalDispatch = dto.Lower5MinLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>'TO SQL'!E34</f>
+        <v>Lower5MinLocalReq</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinLocalReq = dto.Lower5MinLocalReq;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f>'TO SQL'!E35</f>
+        <v>Lower5MinReq</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower5MinReq = dto.Lower5MinReq;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f>'TO SQL'!E36</f>
+        <v>Lower60SecDispatch</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecDispatch = dto.Lower60SecDispatch;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="str">
+        <f>'TO SQL'!E37</f>
+        <v>Lower60SecImport</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecImport = dto.Lower60SecImport;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
+        <f>'TO SQL'!E38</f>
+        <v>Lower60SecLocalDispatch</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecLocalDispatch = dto.Lower60SecLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="str">
+        <f>'TO SQL'!E39</f>
+        <v>Lower60SecLocalReq</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecLocalReq = dto.Lower60SecLocalReq;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="str">
+        <f>'TO SQL'!E40</f>
+        <v>Lower60SecReq</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower60SecReq = dto.Lower60SecReq;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f>'TO SQL'!E41</f>
+        <v>Lower6SecDispatch</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecDispatch = dto.Lower6SecDispatch;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f>'TO SQL'!E42</f>
+        <v>Lower6SecImport</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecImport = dto.Lower6SecImport;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="str">
+        <f>'TO SQL'!E43</f>
+        <v>Lower6SecLocalDispatch</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecLocalDispatch = dto.Lower6SecLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="str">
+        <f>'TO SQL'!E44</f>
+        <v>Lower6SecLocalReq</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecLocalReq = dto.Lower6SecLocalReq;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="str">
+        <f>'TO SQL'!E45</f>
+        <v>Lower6SecReq</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower6SecReq = dto.Lower6SecReq;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
+        <f>'TO SQL'!E46</f>
+        <v>Raise5MinDispatch</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinDispatch = dto.Raise5MinDispatch;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="str">
+        <f>'TO SQL'!E47</f>
+        <v>Raise5MinImport</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinImport = dto.Raise5MinImport;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f>'TO SQL'!E48</f>
+        <v>Raise5MinLocalDispatch</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinLocalDispatch = dto.Raise5MinLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f>'TO SQL'!E49</f>
+        <v>Raise5MinLocalReq</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinLocalReq = dto.Raise5MinLocalReq;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="str">
+        <f>'TO SQL'!E50</f>
+        <v>Raise5MinReq</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise5MinReq = dto.Raise5MinReq;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f>'TO SQL'!E51</f>
+        <v>Raise60SecDispatch</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecDispatch = dto.Raise60SecDispatch;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="str">
+        <f>'TO SQL'!E52</f>
+        <v>Raise60SecImport</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecImport = dto.Raise60SecImport;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="str">
+        <f>'TO SQL'!E53</f>
+        <v>Raise60SecLocalDispatch</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecLocalDispatch = dto.Raise60SecLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="str">
+        <f>'TO SQL'!E54</f>
+        <v>Raise60SecLocalReq</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecLocalReq = dto.Raise60SecLocalReq;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="str">
+        <f>'TO SQL'!E55</f>
+        <v>Raise60SecReq</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise60SecReq = dto.Raise60SecReq;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="str">
+        <f>'TO SQL'!E56</f>
+        <v>Raise6SecDispatch</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecDispatch = dto.Raise6SecDispatch;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f>'TO SQL'!E57</f>
+        <v>Raise6SecImport</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecImport = dto.Raise6SecImport;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="str">
+        <f>'TO SQL'!E58</f>
+        <v>Raise6SecLocalDispatch</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecLocalDispatch = dto.Raise6SecLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="str">
+        <f>'TO SQL'!E59</f>
+        <v>Raise6SecLocalReq</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecLocalReq = dto.Raise6SecLocalReq;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="str">
+        <f>'TO SQL'!E60</f>
+        <v>Raise6SecReq</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>Raise6SecReq = dto.Raise6SecReq;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f>'TO SQL'!E61</f>
+        <v>AggregateDispatchError</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>AggregateDispatchError = dto.AggregateDispatchError;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="str">
+        <f>'TO SQL'!E62</f>
+        <v>InitialSupply</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>InitialSupply = dto.InitialSupply;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="str">
+        <f>'TO SQL'!E63</f>
+        <v>ClearedSupply</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>ClearedSupply = dto.ClearedSupply;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f>'TO SQL'!E64</f>
+        <v>LowerRegImport</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>LowerRegImport = dto.LowerRegImport;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f>'TO SQL'!E65</f>
+        <v>LowerRegDispatch</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>LowerRegDispatch = dto.LowerRegDispatch;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="str">
+        <f>'TO SQL'!E66</f>
+        <v>LowerRegLocalDispatch</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>LowerRegLocalDispatch = dto.LowerRegLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="str">
+        <f>'TO SQL'!E67</f>
+        <v>LowerRegLocalReq</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B104" si="1">_xlfn.CONCAT(A67," = ","dto.",A67,";")</f>
+        <v>LowerRegLocalReq = dto.LowerRegLocalReq;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="str">
+        <f>'TO SQL'!E68</f>
+        <v>LowerRegReq</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>LowerRegReq = dto.LowerRegReq;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="str">
+        <f>'TO SQL'!E69</f>
+        <v>RaiseRegImport</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegImport = dto.RaiseRegImport;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="str">
+        <f>'TO SQL'!E70</f>
+        <v>RaiseRegDispatch</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegDispatch = dto.RaiseRegDispatch;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="str">
+        <f>'TO SQL'!E71</f>
+        <v>RaiseRegLocalDispatch</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegLocalDispatch = dto.RaiseRegLocalDispatch;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="str">
+        <f>'TO SQL'!E72</f>
+        <v>RaiseRegLocalReq</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegLocalReq = dto.RaiseRegLocalReq;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="str">
+        <f>'TO SQL'!E73</f>
+        <v>RaiseRegReq</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegReq = dto.RaiseRegReq;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="str">
+        <f>'TO SQL'!E74</f>
+        <v>Raise5MinLocalViolation</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise5MinLocalViolation = dto.Raise5MinLocalViolation;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="str">
+        <f>'TO SQL'!E75</f>
+        <v>RaiseRegLocalViolation</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegLocalViolation = dto.RaiseRegLocalViolation;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f>'TO SQL'!E76</f>
+        <v>Raise60SecLocalViolation</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise60SecLocalViolation = dto.Raise60SecLocalViolation;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="str">
+        <f>'TO SQL'!E77</f>
+        <v>Raise6SecLocalViolation</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise6SecLocalViolation = dto.Raise6SecLocalViolation;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="str">
+        <f>'TO SQL'!E78</f>
+        <v>Lower5MinLocalViolation</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower5MinLocalViolation = dto.Lower5MinLocalViolation;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="str">
+        <f>'TO SQL'!E79</f>
+        <v>LowerRegLocalViolation</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>LowerRegLocalViolation = dto.LowerRegLocalViolation;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="str">
+        <f>'TO SQL'!E80</f>
+        <v>Lower60SecLocalViolation</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower60SecLocalViolation = dto.Lower60SecLocalViolation;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="str">
+        <f>'TO SQL'!E81</f>
+        <v>Lower6SecLocalViolation</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower6SecLocalViolation = dto.Lower6SecLocalViolation;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="str">
+        <f>'TO SQL'!E82</f>
+        <v>Raise5MinViolation</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise5MinViolation = dto.Raise5MinViolation;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="str">
+        <f>'TO SQL'!E83</f>
+        <v>RaiseRegViolation</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>RaiseRegViolation = dto.RaiseRegViolation;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="str">
+        <f>'TO SQL'!E84</f>
+        <v>Raise60SecViolation</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise60SecViolation = dto.Raise60SecViolation;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="str">
+        <f>'TO SQL'!E85</f>
+        <v>Raise6SecViolation</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>Raise6SecViolation = dto.Raise6SecViolation;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="str">
+        <f>'TO SQL'!E86</f>
+        <v>Lower5MinViolation</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower5MinViolation = dto.Lower5MinViolation;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="str">
+        <f>'TO SQL'!E87</f>
+        <v>LowerRegViolation</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>LowerRegViolation = dto.LowerRegViolation;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="str">
+        <f>'TO SQL'!E88</f>
+        <v>Lower60SecViolation</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower60SecViolation = dto.Lower60SecViolation;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="str">
+        <f>'TO SQL'!E89</f>
+        <v>Lower6SecViolation</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower6SecViolation = dto.Lower6SecViolation;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="str">
+        <f>'TO SQL'!E90</f>
+        <v>LastChanged</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>LastChanged = dto.LastChanged;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="str">
+        <f>'TO SQL'!E91</f>
+        <v>TotalIntermittentGeneration</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>TotalIntermittentGeneration = dto.TotalIntermittentGeneration;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="str">
+        <f>'TO SQL'!E92</f>
+        <v>DemandAndNonSchedgen</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>DemandAndNonSchedgen = dto.DemandAndNonSchedgen;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="str">
+        <f>'TO SQL'!E93</f>
+        <v>Uigf</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>Uigf = dto.Uigf;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="str">
+        <f>'TO SQL'!E94</f>
+        <v>SemiScheduleClearedMw</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>SemiScheduleClearedMw = dto.SemiScheduleClearedMw;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="str">
+        <f>'TO SQL'!E95</f>
+        <v>SemiScheduleComplianceMw</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>SemiScheduleComplianceMw = dto.SemiScheduleComplianceMw;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="str">
+        <f>'TO SQL'!E96</f>
+        <v>SsSolarUigf</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>SsSolarUigf = dto.SsSolarUigf;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="str">
+        <f>'TO SQL'!E97</f>
+        <v>SsWindUigf</v>
+      </c>
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>SsWindUigf = dto.SsWindUigf;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="str">
+        <f>'TO SQL'!E98</f>
+        <v>SsSolarClearedMw</v>
+      </c>
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>SsSolarClearedMw = dto.SsSolarClearedMw;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="str">
+        <f>'TO SQL'!E99</f>
+        <v>SsWindClearedMw</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>SsWindClearedMw = dto.SsWindClearedMw;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="str">
+        <f>'TO SQL'!E100</f>
+        <v>SsSolarComplianceMw</v>
+      </c>
+      <c r="B100" t="str">
+        <f t="shared" si="1"/>
+        <v>SsSolarComplianceMw = dto.SsSolarComplianceMw;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="str">
+        <f>'TO SQL'!E101</f>
+        <v>SsWindComplianceMw</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" si="1"/>
+        <v>SsWindComplianceMw = dto.SsWindComplianceMw;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="str">
+        <f>'TO SQL'!E102</f>
+        <v>WdrInitialMw</v>
+      </c>
+      <c r="B102" t="str">
+        <f t="shared" si="1"/>
+        <v>WdrInitialMw = dto.WdrInitialMw;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="str">
+        <f>'TO SQL'!E103</f>
+        <v>WdrAvailable</v>
+      </c>
+      <c r="B103" t="str">
+        <f t="shared" si="1"/>
+        <v>WdrAvailable = dto.WdrAvailable;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="str">
+        <f>'TO SQL'!E104</f>
+        <v>WdrDispatched</v>
+      </c>
+      <c r="B104" t="str">
+        <f t="shared" si="1"/>
+        <v>WdrDispatched = dto.WdrDispatched;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consistent naming and moving everything to an enum
</commit_message>
<xml_diff>
--- a/Useful/VariableConverted.xlsx
+++ b/Useful/VariableConverted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owenholloway/Code/C#/NemTracker/Useful/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924C8DC-DCA5-9842-BAB4-BA4BF56E0A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5F97A7-38FD-3144-8CC2-B13158A433F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{DA1AE469-F5E3-5145-9063-675D6E6FF3EB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="466">
   <si>
     <t>I</t>
   </si>
@@ -1433,6 +1433,9 @@
   </si>
   <si>
     <t>SemischeduleComplianceMw</t>
+  </si>
+  <si>
+    <t>DISPATCHIS</t>
   </si>
 </sst>
 </file>
@@ -2765,10 +2768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB0BA33-06CC-E248-BE80-0045F320AA22}">
-  <dimension ref="B2:N119"/>
+  <dimension ref="B1:N119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q99" sqref="Q99"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2788,6 +2791,11 @@
     <col min="14" max="14" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>

</xml_diff>